<commit_message>
Committing all the changes till Dec 25th, 2024 includes a working demo project.
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tanya Fauzdar\Selenium4Examples\PropertiesAndUtilities\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E75A08-1017-4D11-921A-152A09FE8CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56E5991-4B7F-4E07-9E0F-1970B1643DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{F98C71DC-9EC7-4219-88D3-9D40A8275F31}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{F98C71DC-9EC7-4219-88D3-9D40A8275F31}"/>
   </bookViews>
   <sheets>
     <sheet name="doLogin" sheetId="2" r:id="rId1"/>
     <sheet name="addCustomer" sheetId="4" r:id="rId2"/>
     <sheet name="findNewCars" sheetId="5" r:id="rId3"/>
-    <sheet name="carNameAndPriceTest" sheetId="6" r:id="rId4"/>
+    <sheet name="carNamesAndCarPricesTest" sheetId="6" r:id="rId4"/>
     <sheet name="doUserReg" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
   <si>
     <t>username</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>BMW Cars</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>audi</t>
@@ -591,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7002ADE2-9047-49E9-B65D-A2E92D24CF16}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="A3:D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -667,7 +664,7 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -678,10 +675,10 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
         <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -691,10 +688,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E23510ED-BE4B-4782-BE0A-B62E558656F0}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -726,7 +723,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -737,10 +734,32 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>